<commit_message>
Modified files after first code review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-carturesti-internship-practice-dispatcher\fwf-carturesti-internship-practice-dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-carturesti-internship-practice-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60598AB6-E8AA-444F-BA4C-8D702109814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED16D1A0-6555-4C02-BF81-1C5CCE6F4EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="585" windowWidth="27975" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -281,9 +281,6 @@
     <t>Title,Author,Price,Language,No Pages</t>
   </si>
   <si>
-    <t>Title,Author,Overall review, No Reviews,Price</t>
-  </si>
-  <si>
     <t>ApplicationProcessName</t>
   </si>
   <si>
@@ -297,6 +294,21 @@
   </si>
   <si>
     <t>This delay will be applied before every activity that selects filters.</t>
+  </si>
+  <si>
+    <t>Title,Author,Overall review,No Reviews,Price</t>
+  </si>
+  <si>
+    <t>Carturesti_Code</t>
+  </si>
+  <si>
+    <t>This will be used as reference when uploading queue items.</t>
+  </si>
+  <si>
+    <t>eMAG_Code</t>
+  </si>
+  <si>
+    <t>This will be used as reference whenn uploading queue items.</t>
   </si>
 </sst>
 </file>
@@ -674,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -798,150 +810,170 @@
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>84</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>82</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" t="s">
-        <v>76</v>
+        <v>93</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
         <v>86</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C32" t="s">
         <v>87</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
         <v>88</v>
       </c>
+      <c r="B34">
+        <v>1.5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>